<commit_message>
Fixed bug in LaboratoryFinding profile.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-LaboratoryFinding.xlsx
+++ b/docs/StructureDefinition-LaboratoryFinding.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="467">
   <si>
     <t>Path</t>
   </si>
@@ -510,6 +510,14 @@
   </si>
   <si>
     <t>Used for filtering what observations are retrieved and displayed.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://aehrc.github.io/genclipr-fhir-ig/CodeSystem/FindingType"/&gt;
+    &lt;code value="laboratory-finding"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>Codes for high level observation categories.</t>
@@ -1322,7 +1330,7 @@
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
     &lt;system value="http://snomed.info/sct"/&gt;
-    &lt;code value="272741003"/&gt;
+    &lt;code value="258755000"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
@@ -3375,7 +3383,7 @@
         <v>45</v>
       </c>
       <c r="R15" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="S15" t="s" s="2">
         <v>45</v>
@@ -3393,10 +3401,10 @@
         <v>79</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3438,10 +3446,10 @@
         <v>45</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3449,11 +3457,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3475,16 +3483,16 @@
         <v>153</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3513,7 +3521,7 @@
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3531,7 +3539,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3546,27 +3554,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3589,19 +3597,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3650,7 +3658,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3665,19 +3673,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3685,7 +3693,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3708,16 +3716,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3767,7 +3775,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3788,13 +3796,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3802,11 +3810,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3825,19 +3833,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3886,7 +3894,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3901,19 +3909,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3921,11 +3929,11 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3944,19 +3952,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -4005,7 +4013,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -4020,19 +4028,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -4040,7 +4048,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -4063,16 +4071,16 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -4122,7 +4130,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -4143,13 +4151,13 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4157,7 +4165,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4180,17 +4188,17 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4239,7 +4247,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4254,19 +4262,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4274,7 +4282,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4297,19 +4305,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4338,7 +4346,7 @@
       </c>
       <c r="X23" s="2"/>
       <c r="Y23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4356,7 +4364,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4365,7 +4373,7 @@
         <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
@@ -4374,24 +4382,24 @@
         <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4417,16 +4425,16 @@
         <v>153</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4451,13 +4459,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4475,7 +4483,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4484,7 +4492,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4499,7 +4507,7 @@
         <v>98</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
@@ -4510,11 +4518,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4536,16 +4544,16 @@
         <v>153</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4570,13 +4578,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4594,7 +4602,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4612,24 +4620,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4652,19 +4660,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4713,7 +4721,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4734,10 +4742,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4748,7 +4756,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4774,13 +4782,13 @@
         <v>153</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4806,13 +4814,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4830,7 +4838,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4848,24 +4856,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4891,16 +4899,16 @@
         <v>153</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4925,13 +4933,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4949,7 +4957,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4970,10 +4978,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4984,7 +4992,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5007,16 +5015,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -5066,7 +5074,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -5084,24 +5092,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5124,16 +5132,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5183,7 +5191,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5201,24 +5209,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5241,19 +5249,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5302,7 +5310,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5314,7 +5322,7 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>45</v>
@@ -5323,10 +5331,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5337,7 +5345,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5363,10 +5371,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5417,7 +5425,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5441,7 +5449,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5452,7 +5460,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5481,7 +5489,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5534,7 +5542,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5558,7 +5566,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5569,11 +5577,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5595,10 +5603,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5653,7 +5661,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5688,7 +5696,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5711,13 +5719,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5768,7 +5776,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5777,7 +5785,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5789,10 +5797,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5803,7 +5811,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5826,13 +5834,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5883,7 +5891,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5892,7 +5900,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5904,10 +5912,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5918,7 +5926,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5944,16 +5952,16 @@
         <v>153</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5981,10 +5989,10 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -6002,7 +6010,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6020,13 +6028,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -6037,7 +6045,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6063,16 +6071,16 @@
         <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -6097,13 +6105,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -6121,7 +6129,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6139,13 +6147,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6156,7 +6164,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6179,17 +6187,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6238,7 +6246,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6262,7 +6270,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6273,7 +6281,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6299,10 +6307,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6353,7 +6361,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6374,10 +6382,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6388,7 +6396,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6411,16 +6419,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6470,7 +6478,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6491,10 +6499,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6505,7 +6513,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6528,16 +6536,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6587,7 +6595,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6608,10 +6616,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6622,7 +6630,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6645,19 +6653,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6694,19 +6702,19 @@
         <v>45</v>
       </c>
       <c r="AA43" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AB43" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AC43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD43" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6727,10 +6735,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6741,7 +6749,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6767,10 +6775,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6821,7 +6829,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6845,7 +6853,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6856,7 +6864,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6885,7 +6893,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6938,7 +6946,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6962,7 +6970,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6973,11 +6981,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6999,10 +7007,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -7057,7 +7065,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7092,7 +7100,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7118,16 +7126,16 @@
         <v>153</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7152,13 +7160,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -7176,7 +7184,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7194,16 +7202,16 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7211,7 +7219,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7234,19 +7242,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7295,7 +7303,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7313,24 +7321,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7356,16 +7364,16 @@
         <v>153</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7390,13 +7398,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7414,7 +7422,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7423,7 +7431,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7438,7 +7446,7 @@
         <v>98</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7449,11 +7457,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7475,16 +7483,16 @@
         <v>153</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7509,13 +7517,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7533,7 +7541,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7551,24 +7559,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7594,16 +7602,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7652,7 +7660,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7673,10 +7681,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7687,10 +7695,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C52" t="s" s="2">
         <v>45</v>
@@ -7712,19 +7720,19 @@
         <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7773,7 +7781,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7794,10 +7802,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7808,7 +7816,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7834,10 +7842,10 @@
         <v>57</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7888,7 +7896,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7912,7 +7920,7 @@
         <v>45</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -7923,7 +7931,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7952,7 +7960,7 @@
         <v>102</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>104</v>
@@ -8005,7 +8013,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8029,7 +8037,7 @@
         <v>45</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8040,11 +8048,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -8066,10 +8074,10 @@
         <v>101</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>104</v>
@@ -8124,7 +8132,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8159,7 +8167,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8185,16 +8193,16 @@
         <v>153</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8204,7 +8212,7 @@
         <v>45</v>
       </c>
       <c r="R56" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>45</v>
@@ -8219,13 +8227,13 @@
         <v>45</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>45</v>
@@ -8243,7 +8251,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>55</v>
@@ -8261,16 +8269,16 @@
         <v>45</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>45</v>
@@ -8278,7 +8286,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8301,19 +8309,19 @@
         <v>56</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>45</v>
@@ -8350,17 +8358,17 @@
         <v>45</v>
       </c>
       <c r="AA57" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AB57" s="2"/>
       <c r="AC57" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD57" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8378,27 +8386,27 @@
         <v>45</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C58" t="s" s="2">
         <v>45</v>
@@ -8420,19 +8428,19 @@
         <v>56</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8481,7 +8489,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8499,24 +8507,24 @@
         <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8542,10 +8550,10 @@
         <v>57</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8596,7 +8604,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8620,7 +8628,7 @@
         <v>45</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8631,7 +8639,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8660,7 +8668,7 @@
         <v>102</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>104</v>
@@ -8701,19 +8709,19 @@
         <v>45</v>
       </c>
       <c r="AA60" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AB60" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AC60" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD60" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8737,7 +8745,7 @@
         <v>45</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
@@ -8748,7 +8756,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8771,19 +8779,19 @@
         <v>56</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -8832,7 +8840,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -8853,10 +8861,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -8867,7 +8875,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8893,20 +8901,20 @@
         <v>75</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P62" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="Q62" t="s" s="2">
         <v>45</v>
@@ -8930,10 +8938,10 @@
         <v>144</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>45</v>
@@ -8951,7 +8959,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -8972,10 +8980,10 @@
         <v>45</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>
@@ -8986,7 +8994,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9012,14 +9020,14 @@
         <v>57</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>45</v>
@@ -9029,7 +9037,7 @@
         <v>45</v>
       </c>
       <c r="R63" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="S63" t="s" s="2">
         <v>45</v>
@@ -9068,7 +9076,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -9089,10 +9097,10 @@
         <v>45</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>45</v>
@@ -9103,7 +9111,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9129,14 +9137,14 @@
         <v>69</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
@@ -9146,7 +9154,7 @@
         <v>45</v>
       </c>
       <c r="R64" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="S64" t="s" s="2">
         <v>45</v>
@@ -9185,7 +9193,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9194,7 +9202,7 @@
         <v>55</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>67</v>
@@ -9206,10 +9214,10 @@
         <v>45</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9220,7 +9228,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9246,16 +9254,16 @@
         <v>75</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>45</v>
@@ -9265,7 +9273,7 @@
         <v>45</v>
       </c>
       <c r="R65" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="S65" t="s" s="2">
         <v>45</v>
@@ -9304,7 +9312,7 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
@@ -9325,10 +9333,10 @@
         <v>45</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
@@ -9339,7 +9347,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9365,16 +9373,16 @@
         <v>153</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>45</v>
@@ -9399,13 +9407,13 @@
         <v>45</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>45</v>
@@ -9423,7 +9431,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
@@ -9432,7 +9440,7 @@
         <v>55</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>67</v>
@@ -9447,7 +9455,7 @@
         <v>98</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>45</v>
@@ -9458,11 +9466,11 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
@@ -9484,16 +9492,16 @@
         <v>153</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
@@ -9518,13 +9526,13 @@
         <v>45</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X67" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y67" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>45</v>
@@ -9542,7 +9550,7 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9560,24 +9568,24 @@
         <v>45</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9603,16 +9611,16 @@
         <v>45</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>45</v>
@@ -9661,7 +9669,7 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
@@ -9682,10 +9690,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>

</xml_diff>